<commit_message>
Updated GDP scaling factor for geoeng/DACD
</commit_message>
<xml_diff>
--- a/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
+++ b/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\Desktop\eps-us develop DACD\InputData\geoeng\DACD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\geoeng\DACD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8892B8-96C3-4622-86C1-F6762CE95593}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23415" windowHeight="10875"/>
+    <workbookView xWindow="38400" yWindow="3855" windowWidth="20955" windowHeight="14370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,17 +19,26 @@
     <sheet name="DACD-energyintensity" sheetId="5" r:id="rId4"/>
     <sheet name="DACD-capex" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>Sources:</t>
   </si>
@@ -147,27 +157,15 @@
     <t>to date.</t>
   </si>
   <si>
-    <t>U.S. GDP</t>
-  </si>
-  <si>
     <t>World GDP</t>
   </si>
   <si>
     <t>trillion USD</t>
   </si>
   <si>
-    <t>trillion UDS</t>
-  </si>
-  <si>
-    <t>US GDP share</t>
-  </si>
-  <si>
     <t>Global DAC Potential</t>
   </si>
   <si>
-    <t>U.S. DAC potential</t>
-  </si>
-  <si>
     <t>Converting to metric tons:</t>
   </si>
   <si>
@@ -289,12 +287,33 @@
   </si>
   <si>
     <t>Amortized CapEx and OM Cost Notes</t>
+  </si>
+  <si>
+    <t>EU and World GDP</t>
+  </si>
+  <si>
+    <t>https://data.worldbank.org/indicator/NY.GDP.MKTP.CD</t>
+  </si>
+  <si>
+    <t>World Bank</t>
+  </si>
+  <si>
+    <t>GDP (current US$) data</t>
+  </si>
+  <si>
+    <t>EU GDP</t>
+  </si>
+  <si>
+    <t>EU GDP share</t>
+  </si>
+  <si>
+    <t>EU DAC potential</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -438,7 +457,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -478,11 +503,17 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>74543</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>43244</xdr:rowOff>
+      <xdr:rowOff>48006</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -776,33 +807,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" customWidth="1"/>
+    <col min="2" max="2" width="47.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,154 +843,177 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="7">
         <v>2019</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B14" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>85</v>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId3" xr:uid="{C788F792-B953-4F6F-913E-5590C7922F89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
+    <col min="2" max="8" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -966,7 +1022,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -977,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -988,7 +1044,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1055,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1010,12 +1066,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1037,7 +1093,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1048,17 +1104,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1080,7 +1136,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1091,34 +1147,34 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -1128,27 +1184,27 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B57">
         <v>2045</v>
       </c>
@@ -1171,7 +1227,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -1197,7 +1253,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -1223,7 +1279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +1287,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B63">
         <v>2045</v>
       </c>
@@ -1254,7 +1310,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -1287,7 +1343,7 @@
         <v>27.071428571428573</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -1320,66 +1376,66 @@
         <v>2.8571428571428568</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72">
+        <v>15.625999999999999</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>39</v>
       </c>
-      <c r="B72">
-        <v>19.39</v>
-      </c>
-      <c r="C72" t="s">
-        <v>41</v>
-      </c>
-      <c r="D72">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>87.799000000000007</v>
+      </c>
+      <c r="C73" t="s">
         <v>40</v>
       </c>
-      <c r="B73">
-        <v>80</v>
-      </c>
-      <c r="C73" t="s">
-        <v>42</v>
-      </c>
       <c r="D73">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B74" s="10">
         <f>B72/B73</f>
-        <v>0.24237500000000001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.17797469219467191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="5" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -1389,7 +1445,7 @@
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>2045</v>
       </c>
@@ -1412,7 +1468,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -1422,30 +1478,30 @@
       </c>
       <c r="C78" s="8">
         <f t="shared" ref="C78:H79" si="1">C64*$B$74</f>
-        <v>8.6562499999999987E-2</v>
+        <v>6.3562390069525673E-2</v>
       </c>
       <c r="D78" s="8">
         <f t="shared" si="1"/>
-        <v>0.34624999999999995</v>
+        <v>0.25424956027810269</v>
       </c>
       <c r="E78" s="8">
         <f t="shared" si="1"/>
-        <v>2.1121250000000003</v>
+        <v>1.5509223176964269</v>
       </c>
       <c r="F78" s="8">
         <f t="shared" si="1"/>
-        <v>6.7172500000000008</v>
+        <v>4.9324414693951928</v>
       </c>
       <c r="G78" s="8">
         <f t="shared" si="1"/>
-        <v>6.6479999999999997</v>
+        <v>4.8815915573395721</v>
       </c>
       <c r="H78" s="8">
-        <f t="shared" si="1"/>
-        <v>6.5614375000000003</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <f>H64*$B$74</f>
+        <v>4.8180291672700468</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -1463,27 +1519,27 @@
       </c>
       <c r="E79" s="8">
         <f t="shared" si="1"/>
-        <v>8.6562499999999987E-2</v>
+        <v>6.3562390069525673E-2</v>
       </c>
       <c r="F79" s="8">
         <f t="shared" si="1"/>
-        <v>0.51937500000000003</v>
+        <v>0.38137434041715407</v>
       </c>
       <c r="G79" s="8">
         <f t="shared" si="1"/>
-        <v>0.60593750000000002</v>
+        <v>0.44493673048667975</v>
       </c>
       <c r="H79" s="8">
-        <f t="shared" si="1"/>
-        <v>0.69249999999999989</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <f>H65*$B$74</f>
+        <v>0.50849912055620539</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>2045</v>
       </c>
@@ -1506,9 +1562,9 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B83" s="12">
         <f>B78*10^9</f>
@@ -1516,32 +1572,32 @@
       </c>
       <c r="C83" s="13">
         <f t="shared" ref="C83:H84" si="2">C78*10^9</f>
-        <v>86562499.999999985</v>
+        <v>63562390.069525674</v>
       </c>
       <c r="D83" s="13">
         <f t="shared" si="2"/>
-        <v>346249999.99999994</v>
+        <v>254249560.2781027</v>
       </c>
       <c r="E83" s="13">
         <f t="shared" si="2"/>
-        <v>2112125000.0000002</v>
+        <v>1550922317.6964269</v>
       </c>
       <c r="F83" s="13">
         <f t="shared" si="2"/>
-        <v>6717250000.000001</v>
+        <v>4932441469.3951931</v>
       </c>
       <c r="G83" s="13">
         <f t="shared" si="2"/>
-        <v>6648000000</v>
+        <v>4881591557.339572</v>
       </c>
       <c r="H83" s="13">
         <f t="shared" si="2"/>
-        <v>6561437500</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4818029167.2700472</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B84" s="12">
         <f>B79*10^9</f>
@@ -1557,57 +1613,57 @@
       </c>
       <c r="E84" s="13">
         <f t="shared" si="2"/>
-        <v>86562499.999999985</v>
+        <v>63562390.069525674</v>
       </c>
       <c r="F84" s="13">
         <f t="shared" si="2"/>
-        <v>519375000.00000006</v>
+        <v>381374340.41715407</v>
       </c>
       <c r="G84" s="13">
         <f t="shared" si="2"/>
-        <v>605937500</v>
+        <v>444936730.48667973</v>
       </c>
       <c r="H84" s="13">
         <f t="shared" si="2"/>
-        <v>692499999.99999988</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>508499120.55620539</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>55</v>
       </c>
       <c r="B92">
         <v>947086</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +1674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1626,15 +1682,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4">
         <v>2017</v>
@@ -1739,9 +1795,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1829,27 +1885,27 @@
       </c>
       <c r="AD2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AD$1)</f>
-        <v>0</v>
+        <v>3.814697265625E-6</v>
       </c>
       <c r="AE2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AE$1)</f>
-        <v>17312500</v>
+        <v>12712478.013908386</v>
       </c>
       <c r="AF2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AF$1)</f>
-        <v>34625000</v>
+        <v>25424956.027812958</v>
       </c>
       <c r="AG2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AG$1)</f>
-        <v>51937500</v>
+        <v>38137434.041717529</v>
       </c>
       <c r="AH2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AH$1)</f>
-        <v>69250000</v>
+        <v>50849912.055622101</v>
       </c>
       <c r="AI2">
         <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AI$1)</f>
-        <v>86562500</v>
+        <v>63562390.069526672</v>
       </c>
     </row>
   </sheetData>
@@ -1858,23 +1914,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4">
         <v>2017</v>
@@ -1979,9 +2037,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="14">
         <f>Data!B16*Data!B92</f>
@@ -2120,9 +2178,9 @@
         <v>1704754.8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2260,9 +2318,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B4" s="14">
         <f>Data!B22*Data!B92</f>
@@ -2401,9 +2459,9 @@
         <v>7671396.5999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2541,9 +2599,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2681,9 +2739,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2821,9 +2879,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2961,9 +3019,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3101,9 +3159,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3241,9 +3299,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3387,23 +3445,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4">
         <v>2017</v>
@@ -3508,9 +3568,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="14">
         <f>Data!B10</f>

</xml_diff>